<commit_message>
updated scheduling algorithm so that all tutors (in Fall2017 sample data) work consecutive shifts (i.e. no 1 hour shifts) and all tutors don't work more than 2 hours at a time
</commit_message>
<xml_diff>
--- a/Sample Data/Fall2017Availability.xlsx
+++ b/Sample Data/Fall2017Availability.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samberling/OneDrive/School/Spring 2018/CSCI 440/Schedule Generator/Sample Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0ED10DA2-FA8F-1C4F-98F0-E151F27E6C06}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E5CF9A-48E2-234D-BECF-26A2B9E566C3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16220" windowHeight="21000" xr2:uid="{71D515E7-43FC-794D-8CCB-B2803B57DA0E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{71D515E7-43FC-794D-8CCB-B2803B57DA0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Fall2017Availability" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -735,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D71848E-EFA5-494B-8942-CEECAAF65D58}">
   <dimension ref="A1:BH45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="BI33" sqref="BI33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>